<commit_message>
DBOM SU - complete v1.0
</commit_message>
<xml_diff>
--- a/CR - Cost Report/2_CBOM/Liste CBOM DBOM.xlsx
+++ b/CR - Cost Report/2_CBOM/Liste CBOM DBOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53afe52601393161/EPSA/Saison 2020/COST/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thilv\Desktop\EPSA\STUF-2020\CR - Cost Report\2_CBOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{FB6374BA-9CE5-4805-A9CC-1E64C3F63C99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E2D525FF-0A66-4733-92FB-C258E5A7D94D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F4DF4B-494C-4B94-9D00-6AAAC65AAAA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14310" yWindow="4050" windowWidth="21600" windowHeight="10995" xr2:uid="{B4482897-36D7-4D63-B03A-E0506F4CBE66}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{B4482897-36D7-4D63-B03A-E0506F4CBE66}"/>
   </bookViews>
   <sheets>
     <sheet name="Fastener" sheetId="2" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FED3E85-6449-4123-886B-7B0EE3FEB009}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>